<commit_message>
modified test case web, add test case Masuk
</commit_message>
<xml_diff>
--- a/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
+++ b/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdil\Downloads\Binar\Challenge Binar Platinum\qae-21-platinum-tima\secondhand-web\test-case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB77FC1F-F621-4C00-BC2E-20E25F0C615D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9D0588-864C-40A5-AF67-CDB472BA1389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="265">
   <si>
     <t>No</t>
   </si>
@@ -748,13 +748,101 @@
   </si>
   <si>
     <t>Klik "Daftar"</t>
+  </si>
+  <si>
+    <t>Masuk</t>
+  </si>
+  <si>
+    <t>Login dengan akun yang valid</t>
+  </si>
+  <si>
+    <t>Memastikan user dapat login dengan akun yang didaftarkan</t>
+  </si>
+  <si>
+    <t>Masukkan Email</t>
+  </si>
+  <si>
+    <t>- Buka halaman Daftar website Secnodhand
+- Memiliki akun yang sudah didaftarkan</t>
+  </si>
+  <si>
+    <t>Masukkan Password</t>
+  </si>
+  <si>
+    <t>Klik Masuk</t>
+  </si>
+  <si>
+    <t>Login dengan email yang tidak valid</t>
+  </si>
+  <si>
+    <t>Memastikan user tidak dapat login dengan email yang tidak terdaftar</t>
+  </si>
+  <si>
+    <t>- Buka halaman Daftar website secnodHand
+- Memiliki akun yang sudah didaftarkan</t>
+  </si>
+  <si>
+    <t>Menampilkan alert "Invalid Email or password."</t>
+  </si>
+  <si>
+    <t>Login dengan passwword yang tidak valid</t>
+  </si>
+  <si>
+    <t>Memastikan user tidak dapat login dengan password yang tidak terdaftar</t>
+  </si>
+  <si>
+    <t>- Buka halaman Masuk website secnodHand
+- Memiliki akun yang sudah diMasukkan</t>
+  </si>
+  <si>
+    <t>Login dengan email yang tidak sesuai format</t>
+  </si>
+  <si>
+    <t>Memastikan alert field email wajib menambahkan @</t>
+  </si>
+  <si>
+    <t>Inputfield Email tanpa @</t>
+  </si>
+  <si>
+    <t>Menampilkan alert "Please include an '@' in the email address. 'aaaa' is missing an '@'."</t>
+  </si>
+  <si>
+    <t>- Buka halaman login website secnodHand
+- Memiliki akun yang sudah didaftarkan</t>
+  </si>
+  <si>
+    <t>Input data Field Password</t>
+  </si>
+  <si>
+    <t>Gagal masuk ke halaman dashboard</t>
+  </si>
+  <si>
+    <t>Tampilkan halaman Daftar</t>
+  </si>
+  <si>
+    <t>Memastikan "Daftar di sini" mengarahkan ke halaman Daftar</t>
+  </si>
+  <si>
+    <t>klik "Daftar di sini"</t>
+  </si>
+  <si>
+    <t>Menampilkan halaman Daftar</t>
+  </si>
+  <si>
+    <t>- Buka halaman Masuk website secnodHand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data dapat diinput </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berhasil menamplkan halaman dashboard </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -795,6 +883,25 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -816,7 +923,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -850,11 +957,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -945,6 +1078,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D3FED-4954-4F6C-AB9D-DEFE7553E9DB}">
   <dimension ref="A1:J880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4348,220 +4540,384 @@
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" s="32"/>
-      <c r="B151" s="23"/>
-      <c r="C151" s="23"/>
-      <c r="D151" s="23"/>
-      <c r="E151" s="23"/>
-      <c r="F151" s="32"/>
-      <c r="G151" s="23"/>
-      <c r="H151" s="23"/>
-      <c r="I151" s="23"/>
-      <c r="J151" s="33"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" s="32"/>
-      <c r="B152" s="23"/>
-      <c r="C152" s="23"/>
-      <c r="D152" s="23"/>
-      <c r="E152" s="23"/>
-      <c r="F152" s="32"/>
-      <c r="G152" s="23"/>
-      <c r="H152" s="23"/>
-      <c r="I152" s="23"/>
-      <c r="J152" s="33"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" s="32"/>
-      <c r="B153" s="23"/>
-      <c r="C153" s="23"/>
-      <c r="D153" s="23"/>
-      <c r="E153" s="23"/>
-      <c r="F153" s="32"/>
-      <c r="G153" s="23"/>
-      <c r="H153" s="23"/>
-      <c r="I153" s="23"/>
-      <c r="J153" s="33"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A154" s="32"/>
-      <c r="B154" s="23"/>
-      <c r="C154" s="23"/>
-      <c r="D154" s="23"/>
-      <c r="E154" s="23"/>
-      <c r="F154" s="32"/>
-      <c r="G154" s="23"/>
-      <c r="H154" s="23"/>
-      <c r="I154" s="23"/>
-      <c r="J154" s="33"/>
+      <c r="A151" s="34"/>
+      <c r="B151" s="35"/>
+      <c r="C151" s="35"/>
+      <c r="D151" s="35"/>
+      <c r="E151" s="35"/>
+      <c r="F151" s="36"/>
+      <c r="G151" s="35"/>
+      <c r="H151" s="35"/>
+      <c r="I151" s="35"/>
+      <c r="J151" s="34"/>
+    </row>
+    <row r="152" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A152" s="38">
+        <v>36</v>
+      </c>
+      <c r="B152" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C152" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D152" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="E152" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F152" s="40">
+        <v>1</v>
+      </c>
+      <c r="G152" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="H152" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="I152" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="J152" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A153" s="38"/>
+      <c r="B153" s="39"/>
+      <c r="C153" s="39"/>
+      <c r="D153" s="39"/>
+      <c r="E153" s="39"/>
+      <c r="F153" s="40">
+        <v>2</v>
+      </c>
+      <c r="G153" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="H153" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I153" s="39"/>
+      <c r="J153" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="38"/>
+      <c r="B154" s="39"/>
+      <c r="C154" s="39"/>
+      <c r="D154" s="39"/>
+      <c r="E154" s="39"/>
+      <c r="F154" s="40">
+        <v>3</v>
+      </c>
+      <c r="G154" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="H154" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="I154" s="39"/>
+      <c r="J154" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A155" s="32"/>
-      <c r="B155" s="23"/>
-      <c r="C155" s="23"/>
-      <c r="D155" s="23"/>
-      <c r="E155" s="23"/>
-      <c r="F155" s="32"/>
-      <c r="G155" s="23"/>
-      <c r="H155" s="23"/>
-      <c r="I155" s="23"/>
-      <c r="J155" s="33"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156" s="32"/>
-      <c r="B156" s="23"/>
-      <c r="C156" s="23"/>
-      <c r="D156" s="23"/>
-      <c r="E156" s="23"/>
-      <c r="F156" s="32"/>
-      <c r="G156" s="23"/>
-      <c r="H156" s="23"/>
-      <c r="I156" s="23"/>
-      <c r="J156" s="33"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A157" s="32"/>
-      <c r="B157" s="23"/>
-      <c r="C157" s="23"/>
-      <c r="D157" s="23"/>
-      <c r="E157" s="23"/>
-      <c r="F157" s="32"/>
-      <c r="G157" s="23"/>
-      <c r="H157" s="23"/>
-      <c r="I157" s="23"/>
-      <c r="J157" s="33"/>
+      <c r="A155" s="44"/>
+      <c r="B155" s="45"/>
+      <c r="C155" s="45"/>
+      <c r="D155" s="45"/>
+      <c r="E155" s="45"/>
+      <c r="F155" s="46"/>
+      <c r="G155" s="45"/>
+      <c r="H155" s="45"/>
+      <c r="I155" s="45"/>
+      <c r="J155" s="47"/>
+    </row>
+    <row r="156" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A156" s="48">
+        <v>37</v>
+      </c>
+      <c r="B156" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C156" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="E156" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="F156" s="50">
+        <v>1</v>
+      </c>
+      <c r="G156" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="H156" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="I156" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="J156" s="51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A157" s="52"/>
+      <c r="B157" s="53"/>
+      <c r="C157" s="53"/>
+      <c r="D157" s="53"/>
+      <c r="E157" s="53"/>
+      <c r="F157" s="50">
+        <v>2</v>
+      </c>
+      <c r="G157" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="H157" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I157" s="53"/>
+      <c r="J157" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" s="32"/>
-      <c r="B158" s="23"/>
-      <c r="C158" s="23"/>
-      <c r="D158" s="23"/>
-      <c r="E158" s="23"/>
-      <c r="F158" s="32"/>
-      <c r="G158" s="23"/>
-      <c r="H158" s="23"/>
-      <c r="I158" s="23"/>
-      <c r="J158" s="33"/>
+      <c r="A158" s="52"/>
+      <c r="B158" s="53"/>
+      <c r="C158" s="53"/>
+      <c r="D158" s="53"/>
+      <c r="E158" s="53"/>
+      <c r="F158" s="50">
+        <v>3</v>
+      </c>
+      <c r="G158" s="54" t="s">
+        <v>243</v>
+      </c>
+      <c r="H158" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I158" s="53"/>
+      <c r="J158" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159" s="32"/>
-      <c r="B159" s="23"/>
-      <c r="C159" s="23"/>
-      <c r="D159" s="23"/>
-      <c r="E159" s="23"/>
-      <c r="F159" s="32"/>
-      <c r="G159" s="23"/>
-      <c r="H159" s="23"/>
-      <c r="I159" s="23"/>
-      <c r="J159" s="33"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" s="32"/>
-      <c r="B160" s="23"/>
-      <c r="C160" s="23"/>
-      <c r="D160" s="23"/>
-      <c r="E160" s="23"/>
-      <c r="F160" s="32"/>
-      <c r="G160" s="23"/>
-      <c r="H160" s="23"/>
-      <c r="I160" s="23"/>
-      <c r="J160" s="33"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" s="32"/>
-      <c r="B161" s="23"/>
-      <c r="C161" s="23"/>
-      <c r="D161" s="23"/>
-      <c r="E161" s="23"/>
-      <c r="F161" s="32"/>
-      <c r="G161" s="23"/>
-      <c r="H161" s="23"/>
-      <c r="I161" s="23"/>
-      <c r="J161" s="33"/>
+      <c r="A159" s="44"/>
+      <c r="B159" s="45"/>
+      <c r="C159" s="45"/>
+      <c r="D159" s="45"/>
+      <c r="E159" s="45"/>
+      <c r="F159" s="46"/>
+      <c r="G159" s="45"/>
+      <c r="H159" s="45"/>
+      <c r="I159" s="45"/>
+      <c r="J159" s="47"/>
+    </row>
+    <row r="160" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A160" s="48">
+        <v>38</v>
+      </c>
+      <c r="B160" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C160" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="E160" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="F160" s="50">
+        <v>1</v>
+      </c>
+      <c r="G160" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="H160" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="I160" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="J160" s="51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A161" s="52"/>
+      <c r="B161" s="53"/>
+      <c r="C161" s="53"/>
+      <c r="D161" s="53"/>
+      <c r="E161" s="53"/>
+      <c r="F161" s="50">
+        <v>2</v>
+      </c>
+      <c r="G161" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="H161" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I161" s="53"/>
+      <c r="J161" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A162" s="32"/>
-      <c r="B162" s="23"/>
-      <c r="C162" s="23"/>
-      <c r="D162" s="23"/>
-      <c r="E162" s="23"/>
-      <c r="F162" s="32"/>
-      <c r="G162" s="23"/>
-      <c r="H162" s="23"/>
-      <c r="I162" s="23"/>
-      <c r="J162" s="33"/>
+      <c r="A162" s="52"/>
+      <c r="B162" s="53"/>
+      <c r="C162" s="53"/>
+      <c r="D162" s="53"/>
+      <c r="E162" s="53"/>
+      <c r="F162" s="50">
+        <v>3</v>
+      </c>
+      <c r="G162" s="54" t="s">
+        <v>243</v>
+      </c>
+      <c r="H162" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I162" s="53"/>
+      <c r="J162" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A163" s="32"/>
-      <c r="B163" s="23"/>
-      <c r="C163" s="23"/>
-      <c r="D163" s="23"/>
-      <c r="E163" s="23"/>
-      <c r="F163" s="32"/>
-      <c r="G163" s="23"/>
-      <c r="H163" s="23"/>
-      <c r="I163" s="23"/>
-      <c r="J163" s="33"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A164" s="32"/>
-      <c r="B164" s="23"/>
-      <c r="C164" s="23"/>
-      <c r="D164" s="23"/>
-      <c r="E164" s="23"/>
-      <c r="F164" s="32"/>
-      <c r="G164" s="23"/>
-      <c r="H164" s="23"/>
-      <c r="I164" s="23"/>
-      <c r="J164" s="33"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A165" s="32"/>
-      <c r="B165" s="23"/>
-      <c r="C165" s="23"/>
-      <c r="D165" s="23"/>
-      <c r="E165" s="23"/>
-      <c r="F165" s="32"/>
-      <c r="G165" s="23"/>
-      <c r="H165" s="23"/>
-      <c r="I165" s="23"/>
-      <c r="J165" s="33"/>
+      <c r="A163" s="34"/>
+      <c r="B163" s="35"/>
+      <c r="C163" s="35"/>
+      <c r="D163" s="35"/>
+      <c r="E163" s="35"/>
+      <c r="F163" s="36"/>
+      <c r="G163" s="35"/>
+      <c r="H163" s="35"/>
+      <c r="I163" s="35"/>
+      <c r="J163" s="34"/>
+    </row>
+    <row r="164" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A164" s="38">
+        <v>39</v>
+      </c>
+      <c r="B164" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C164" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D164" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="E164" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="F164" s="40">
+        <v>1</v>
+      </c>
+      <c r="G164" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="H164" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="I164" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="J164" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A165" s="38"/>
+      <c r="B165" s="39"/>
+      <c r="C165" s="39"/>
+      <c r="D165" s="39"/>
+      <c r="E165" s="39"/>
+      <c r="F165" s="40">
+        <v>2</v>
+      </c>
+      <c r="G165" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="H165" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I165" s="39"/>
+      <c r="J165" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A166" s="32"/>
-      <c r="B166" s="23"/>
-      <c r="C166" s="23"/>
-      <c r="D166" s="23"/>
-      <c r="E166" s="23"/>
-      <c r="F166" s="32"/>
-      <c r="G166" s="23"/>
-      <c r="H166" s="23"/>
-      <c r="I166" s="23"/>
-      <c r="J166" s="33"/>
+      <c r="A166" s="38"/>
+      <c r="B166" s="39"/>
+      <c r="C166" s="39"/>
+      <c r="D166" s="39"/>
+      <c r="E166" s="39"/>
+      <c r="F166" s="40">
+        <v>3</v>
+      </c>
+      <c r="G166" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="H166" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="I166" s="39"/>
+      <c r="J166" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" s="32"/>
-      <c r="B167" s="23"/>
-      <c r="C167" s="23"/>
-      <c r="D167" s="23"/>
-      <c r="E167" s="23"/>
-      <c r="F167" s="32"/>
-      <c r="G167" s="23"/>
-      <c r="H167" s="23"/>
-      <c r="I167" s="23"/>
-      <c r="J167" s="33"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" s="32"/>
-      <c r="B168" s="23"/>
-      <c r="C168" s="23"/>
-      <c r="D168" s="23"/>
-      <c r="E168" s="23"/>
-      <c r="F168" s="32"/>
-      <c r="G168" s="23"/>
-      <c r="H168" s="23"/>
-      <c r="I168" s="23"/>
-      <c r="J168" s="33"/>
+      <c r="A167" s="34"/>
+      <c r="B167" s="35"/>
+      <c r="C167" s="35"/>
+      <c r="D167" s="35"/>
+      <c r="E167" s="35"/>
+      <c r="F167" s="36"/>
+      <c r="G167" s="35"/>
+      <c r="H167" s="35"/>
+      <c r="I167" s="35"/>
+      <c r="J167" s="34"/>
+    </row>
+    <row r="168" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A168" s="38">
+        <v>40</v>
+      </c>
+      <c r="B168" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="C168" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="E168" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="F168" s="40">
+        <v>1</v>
+      </c>
+      <c r="G168" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="H168" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="I168" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="J168" s="42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="32"/>
@@ -13109,10 +13465,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J5 J7:J10 J12:J15 J17:J19 J21 J23:J26 J28:J29 J31:J32 J34:J38 J40:J49 J51 J53:J54 J58 J60 J62:J68 J70:J76 J78:J79 J81:J84 J86:J90 J92:J96 J98:J101 J105:J108 J110:J113 J115:J119 J121:J125 J127:J131 J133:J137 J139:J141 J143:J144 J146 J148 J150" xr:uid="{ECE8CF73-52E7-4EC9-A9B7-66A7B95BCC7A}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J5 J7:J10 J12:J15 J17:J19 J21 J23:J26 J28:J29 J31:J32 J34:J38 J40:J49 J51 J53:J54 J58 J60 J62:J68 J70:J76 J78:J79 J81:J84 J86:J90 J92:J96 J98:J101 J105:J108 J110:J113 J115:J119 J121:J125 J127:J131 J133:J137 J139:J141 J143:J144 J146 J148 J150 J152:J154 J156:J158 J160:J162 J164:J166 J168" xr:uid="{ECE8CF73-52E7-4EC9-A9B7-66A7B95BCC7A}">
       <formula1>"Ready to Test,Pass,Fail,Block"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2 C7 C12 C17 C21 C23 C28 C31 C34 C40 C46 C51 C53 C56 C58 C60 C62 C70 C78 C81 C86 C92 C98 C103 C105 C110 C115 C121 C127 C133 C139 C143 C146 C148 C150" xr:uid="{C1E65F4A-851E-4DBA-B645-2E5C0BE4A124}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2 C7 C12 C17 C21 C23 C28 C31 C34 C40 C46 C51 C53 C56 C58 C60 C62 C70 C78 C81 C86 C92 C98 C103 C105 C110 C115 C121 C127 C133 C139 C143 C146 C148 C150 C152 C156 C160 C164 C168" xr:uid="{C1E65F4A-851E-4DBA-B645-2E5C0BE4A124}">
       <formula1>"Positive,Negative"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
modified test case web
</commit_message>
<xml_diff>
--- a/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
+++ b/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdil\Downloads\Binar\Challenge Binar Platinum\qae-21-platinum-tima\secondhand-web\test-case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9D0588-864C-40A5-AF67-CDB472BA1389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502B5C1C-D52F-4756-A431-2E1CB6B57EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,9 +756,6 @@
     <t>Login dengan akun yang valid</t>
   </si>
   <si>
-    <t>Memastikan user dapat login dengan akun yang didaftarkan</t>
-  </si>
-  <si>
     <t>Masukkan Email</t>
   </si>
   <si>
@@ -836,6 +833,9 @@
   </si>
   <si>
     <t xml:space="preserve">Berhasil menamplkan halaman dashboard </t>
+  </si>
+  <si>
+    <t>Memastikan user dapat login dengan akun yang sudah didaftarkan</t>
   </si>
 </sst>
 </file>
@@ -1354,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D3FED-4954-4F6C-AB9D-DEFE7553E9DB}">
   <dimension ref="A1:J880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4565,19 +4565,19 @@
         <v>238</v>
       </c>
       <c r="E152" s="39" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="F152" s="40">
         <v>1</v>
       </c>
       <c r="G152" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="H152" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="I152" s="39" t="s">
         <v>240</v>
-      </c>
-      <c r="H152" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="I152" s="39" t="s">
-        <v>241</v>
       </c>
       <c r="J152" s="42" t="s">
         <v>15</v>
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="G153" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H153" s="39" t="s">
         <v>14</v>
@@ -4613,10 +4613,10 @@
         <v>3</v>
       </c>
       <c r="G154" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H154" s="39" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I154" s="39"/>
       <c r="J154" s="42" t="s">
@@ -4646,22 +4646,22 @@
         <v>11</v>
       </c>
       <c r="D156" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E156" s="41" t="s">
         <v>244</v>
-      </c>
-      <c r="E156" s="41" t="s">
-        <v>245</v>
       </c>
       <c r="F156" s="50">
         <v>1</v>
       </c>
       <c r="G156" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H156" s="41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I156" s="39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J156" s="51" t="s">
         <v>15</v>
@@ -4677,7 +4677,7 @@
         <v>2</v>
       </c>
       <c r="G157" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H157" s="41" t="s">
         <v>14</v>
@@ -4697,10 +4697,10 @@
         <v>3</v>
       </c>
       <c r="G158" s="54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H158" s="41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I158" s="53"/>
       <c r="J158" s="51" t="s">
@@ -4730,22 +4730,22 @@
         <v>11</v>
       </c>
       <c r="D160" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="E160" s="41" t="s">
         <v>248</v>
-      </c>
-      <c r="E160" s="41" t="s">
-        <v>249</v>
       </c>
       <c r="F160" s="50">
         <v>1</v>
       </c>
       <c r="G160" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H160" s="41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I160" s="39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J160" s="51" t="s">
         <v>15</v>
@@ -4761,7 +4761,7 @@
         <v>2</v>
       </c>
       <c r="G161" s="41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H161" s="41" t="s">
         <v>14</v>
@@ -4781,10 +4781,10 @@
         <v>3</v>
       </c>
       <c r="G162" s="54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H162" s="41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I162" s="53"/>
       <c r="J162" s="51" t="s">
@@ -4814,22 +4814,22 @@
         <v>19</v>
       </c>
       <c r="D164" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="E164" s="39" t="s">
         <v>251</v>
-      </c>
-      <c r="E164" s="39" t="s">
-        <v>252</v>
       </c>
       <c r="F164" s="40">
         <v>1</v>
       </c>
       <c r="G164" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="H164" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="H164" s="39" t="s">
+      <c r="I164" s="39" t="s">
         <v>254</v>
-      </c>
-      <c r="I164" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="J164" s="42" t="s">
         <v>15</v>
@@ -4845,7 +4845,7 @@
         <v>2</v>
       </c>
       <c r="G165" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H165" s="39" t="s">
         <v>14</v>
@@ -4865,10 +4865,10 @@
         <v>3</v>
       </c>
       <c r="G166" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H166" s="43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I166" s="39"/>
       <c r="J166" s="42" t="s">
@@ -4898,22 +4898,22 @@
         <v>11</v>
       </c>
       <c r="D168" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="E168" s="39" t="s">
         <v>258</v>
-      </c>
-      <c r="E168" s="39" t="s">
-        <v>259</v>
       </c>
       <c r="F168" s="40">
         <v>1</v>
       </c>
       <c r="G168" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="H168" s="39" t="s">
         <v>260</v>
       </c>
-      <c r="H168" s="39" t="s">
+      <c r="I168" s="39" t="s">
         <v>261</v>
-      </c>
-      <c r="I168" s="39" t="s">
-        <v>262</v>
       </c>
       <c r="J168" s="42" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
improvements to web test cases
</commit_message>
<xml_diff>
--- a/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
+++ b/secondhand-web/test-case/Test Scenario - SecondHand- web-tima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdil\Downloads\Binar\Challenge Binar Platinum\qae-21-platinum-tima\secondhand-web\test-case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502B5C1C-D52F-4756-A431-2E1CB6B57EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10942D5-C2D7-4BC5-9321-C579FA1A736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="264">
   <si>
     <t>No</t>
   </si>
@@ -756,16 +756,10 @@
     <t>Login dengan akun yang valid</t>
   </si>
   <si>
-    <t>Masukkan Email</t>
-  </si>
-  <si>
     <t>- Buka halaman Daftar website Secnodhand
 - Memiliki akun yang sudah didaftarkan</t>
   </si>
   <si>
-    <t>Masukkan Password</t>
-  </si>
-  <si>
     <t>Klik Masuk</t>
   </si>
   <si>
@@ -798,9 +792,6 @@
     <t>Memastikan alert field email wajib menambahkan @</t>
   </si>
   <si>
-    <t>Inputfield Email tanpa @</t>
-  </si>
-  <si>
     <t>Menampilkan alert "Please include an '@' in the email address. 'aaaa' is missing an '@'."</t>
   </si>
   <si>
@@ -808,9 +799,6 @@
 - Memiliki akun yang sudah didaftarkan</t>
   </si>
   <si>
-    <t>Input data Field Password</t>
-  </si>
-  <si>
     <t>Gagal masuk ke halaman dashboard</t>
   </si>
   <si>
@@ -836,6 +824,15 @@
   </si>
   <si>
     <t>Memastikan user dapat login dengan akun yang sudah didaftarkan</t>
+  </si>
+  <si>
+    <t>Klik "Masuk"</t>
+  </si>
+  <si>
+    <t>Inputfield "Email" tanpa @</t>
+  </si>
+  <si>
+    <t>Input data Field "Password"</t>
   </si>
 </sst>
 </file>
@@ -1354,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D3FED-4954-4F6C-AB9D-DEFE7553E9DB}">
   <dimension ref="A1:J880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E154" sqref="E154"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H168" sqref="H168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3189,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="14" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="H86" s="14" t="s">
         <v>37</v>
@@ -4565,19 +4562,19 @@
         <v>238</v>
       </c>
       <c r="E152" s="39" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F152" s="40">
         <v>1</v>
       </c>
       <c r="G152" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H152" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="I152" s="39" t="s">
         <v>239</v>
-      </c>
-      <c r="H152" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="I152" s="39" t="s">
-        <v>240</v>
       </c>
       <c r="J152" s="42" t="s">
         <v>15</v>
@@ -4593,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="G153" s="41" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="H153" s="39" t="s">
         <v>14</v>
@@ -4613,10 +4610,10 @@
         <v>3</v>
       </c>
       <c r="G154" s="43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H154" s="39" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I154" s="39"/>
       <c r="J154" s="42" t="s">
@@ -4646,22 +4643,22 @@
         <v>11</v>
       </c>
       <c r="D156" s="41" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E156" s="41" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F156" s="50">
         <v>1</v>
       </c>
       <c r="G156" s="41" t="s">
-        <v>239</v>
+        <v>16</v>
       </c>
       <c r="H156" s="41" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I156" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J156" s="51" t="s">
         <v>15</v>
@@ -4677,7 +4674,7 @@
         <v>2</v>
       </c>
       <c r="G157" s="41" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="H157" s="41" t="s">
         <v>14</v>
@@ -4697,10 +4694,10 @@
         <v>3</v>
       </c>
       <c r="G158" s="54" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="H158" s="41" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I158" s="53"/>
       <c r="J158" s="51" t="s">
@@ -4730,22 +4727,22 @@
         <v>11</v>
       </c>
       <c r="D160" s="41" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E160" s="41" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F160" s="50">
         <v>1</v>
       </c>
       <c r="G160" s="41" t="s">
-        <v>239</v>
+        <v>16</v>
       </c>
       <c r="H160" s="41" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I160" s="39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J160" s="51" t="s">
         <v>15</v>
@@ -4761,7 +4758,7 @@
         <v>2</v>
       </c>
       <c r="G161" s="41" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="H161" s="41" t="s">
         <v>14</v>
@@ -4781,10 +4778,10 @@
         <v>3</v>
       </c>
       <c r="G162" s="54" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="H162" s="41" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I162" s="53"/>
       <c r="J162" s="51" t="s">
@@ -4814,22 +4811,22 @@
         <v>19</v>
       </c>
       <c r="D164" s="39" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E164" s="39" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F164" s="40">
         <v>1</v>
       </c>
       <c r="G164" s="39" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="H164" s="39" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I164" s="39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J164" s="42" t="s">
         <v>15</v>
@@ -4845,7 +4842,7 @@
         <v>2</v>
       </c>
       <c r="G165" s="39" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="H165" s="39" t="s">
         <v>14</v>
@@ -4865,10 +4862,10 @@
         <v>3</v>
       </c>
       <c r="G166" s="43" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="H166" s="43" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I166" s="39"/>
       <c r="J166" s="42" t="s">
@@ -4898,22 +4895,22 @@
         <v>11</v>
       </c>
       <c r="D168" s="39" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E168" s="39" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F168" s="40">
         <v>1</v>
       </c>
       <c r="G168" s="39" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H168" s="39" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="I168" s="39" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="J168" s="42" t="s">
         <v>15</v>

</xml_diff>